<commit_message>
Converter gibt XML-Temp-Datei nun aus
</commit_message>
<xml_diff>
--- a/Customizing/global/plugins/Services/UIComponent/UserInterfaceHook/CourseImport/resources/ILIASKursImport_Template.xlsx
+++ b/Customizing/global/plugins/Services/UIComponent/UserInterfaceHook/CourseImport/resources/ILIASKursImport_Template.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manuel\SkyDrive\Dokumente\StuPro\IZIS\iliasVO\Customizing\global\plugins\Services\UIComponent\UserInterfaceHook\CourseImport\resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11850"/>
   </bookViews>
@@ -31,7 +26,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -58,7 +53,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -84,7 +79,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -99,7 +94,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0">
+    <comment ref="D1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -125,7 +120,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0">
+    <comment ref="E1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -151,7 +146,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0">
+    <comment ref="F1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -178,7 +173,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0">
+    <comment ref="G1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -205,7 +200,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0">
+    <comment ref="H1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -233,7 +228,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0">
+    <comment ref="I1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -260,7 +255,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0">
+    <comment ref="J1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -286,7 +281,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0">
+    <comment ref="K1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -312,7 +307,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0" shapeId="0">
+    <comment ref="L1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -338,7 +333,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0">
+    <comment ref="M1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -364,7 +359,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0" shapeId="0">
+    <comment ref="N1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -390,7 +385,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0" shapeId="0">
+    <comment ref="O1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -421,7 +416,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="34">
   <si>
     <t>Zahl</t>
   </si>
@@ -523,24 +518,12 @@
   </si>
   <si>
     <t>Gruppe5</t>
-  </si>
-  <si>
-    <t>user1</t>
-  </si>
-  <si>
-    <t>crs | grp</t>
-  </si>
-  <si>
-    <t>Typ</t>
-  </si>
-  <si>
-    <t>grp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
@@ -1918,7 +1901,7 @@
   <dimension ref="A1:P8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1984,9 +1967,7 @@
       <c r="O1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="P1" s="7" t="s">
-        <v>35</v>
-      </c>
+      <c r="P1" s="7"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -2034,13 +2015,11 @@
       <c r="O2" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="P2" s="10" t="s">
-        <v>36</v>
-      </c>
+      <c r="P2" s="10"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>28</v>
@@ -2049,7 +2028,7 @@
         <v>22</v>
       </c>
       <c r="D3">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3" t="s">
@@ -2077,6 +2056,9 @@
       <c r="P3" s="10"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>112</v>
+      </c>
       <c r="B4" s="3" t="s">
         <v>29</v>
       </c>
@@ -2084,11 +2066,11 @@
         <v>29</v>
       </c>
       <c r="D4">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="E4" s="3"/>
-      <c r="F4" s="4" t="s">
-        <v>34</v>
+      <c r="F4" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="G4" t="s">
         <v>24</v>
@@ -2117,11 +2099,12 @@
       <c r="O4" s="9">
         <v>0.99998842592592585</v>
       </c>
-      <c r="P4" s="10" t="s">
-        <v>37</v>
-      </c>
+      <c r="P4" s="10"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>113</v>
+      </c>
       <c r="B5" t="s">
         <v>30</v>
       </c>
@@ -2129,10 +2112,10 @@
         <v>30</v>
       </c>
       <c r="D5">
-        <v>83</v>
-      </c>
-      <c r="F5" t="s">
-        <v>34</v>
+        <v>66</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="G5" t="s">
         <v>24</v>
@@ -2161,11 +2144,12 @@
       <c r="O5" s="9">
         <v>0.99998842592592585</v>
       </c>
-      <c r="P5" s="10" t="s">
-        <v>37</v>
-      </c>
+      <c r="P5" s="10"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>114</v>
+      </c>
       <c r="B6" t="s">
         <v>31</v>
       </c>
@@ -2173,10 +2157,10 @@
         <v>31</v>
       </c>
       <c r="D6">
-        <v>83</v>
-      </c>
-      <c r="F6" t="s">
-        <v>34</v>
+        <v>66</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="G6" t="s">
         <v>24</v>
@@ -2205,11 +2189,12 @@
       <c r="O6" s="9">
         <v>0.99998842592592585</v>
       </c>
-      <c r="P6" s="10" t="s">
-        <v>37</v>
-      </c>
+      <c r="P6" s="10"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>115</v>
+      </c>
       <c r="B7" t="s">
         <v>32</v>
       </c>
@@ -2217,10 +2202,10 @@
         <v>32</v>
       </c>
       <c r="D7">
-        <v>83</v>
-      </c>
-      <c r="F7" t="s">
-        <v>34</v>
+        <v>66</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="G7" t="s">
         <v>24</v>
@@ -2249,11 +2234,12 @@
       <c r="O7" s="9">
         <v>0.99998842592592585</v>
       </c>
-      <c r="P7" s="10" t="s">
-        <v>37</v>
-      </c>
+      <c r="P7" s="10"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>116</v>
+      </c>
       <c r="B8" t="s">
         <v>33</v>
       </c>
@@ -2261,10 +2247,10 @@
         <v>33</v>
       </c>
       <c r="D8">
-        <v>83</v>
-      </c>
-      <c r="F8" t="s">
-        <v>34</v>
+        <v>66</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="G8" t="s">
         <v>24</v>
@@ -2293,9 +2279,7 @@
       <c r="O8" s="9">
         <v>0.99998842592592585</v>
       </c>
-      <c r="P8" s="10" t="s">
-        <v>37</v>
-      </c>
+      <c r="P8" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Typ Gruppe/Kurs in Xls, Converter, Validator und XML eingefügt. TODO: Gruppenerstellung ähnlich der Kurserstellung
</commit_message>
<xml_diff>
--- a/Customizing/global/plugins/Services/UIComponent/UserInterfaceHook/CourseImport/resources/ILIASKursImport_Template.xlsx
+++ b/Customizing/global/plugins/Services/UIComponent/UserInterfaceHook/CourseImport/resources/ILIASKursImport_Template.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16925"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manuel\SkyDrive\Dokumente\StuPro\IZIS\iliasVO\Customizing\global\plugins\Services\UIComponent\UserInterfaceHook\CourseImport\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11850"/>
   </bookViews>
@@ -26,7 +31,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -53,7 +58,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -79,7 +84,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0">
+    <comment ref="C1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -94,7 +99,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0">
+    <comment ref="D1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -120,7 +125,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0">
+    <comment ref="E1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -146,7 +151,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0">
+    <comment ref="F1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -173,7 +178,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0">
+    <comment ref="G1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -200,7 +205,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0">
+    <comment ref="H1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -228,7 +233,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0">
+    <comment ref="I1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -255,7 +260,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0">
+    <comment ref="J1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -281,7 +286,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0">
+    <comment ref="K1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -307,7 +312,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0">
+    <comment ref="L1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -333,7 +338,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0">
+    <comment ref="M1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -359,7 +364,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0">
+    <comment ref="N1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -385,7 +390,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0">
+    <comment ref="O1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -416,7 +421,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="37">
   <si>
     <t>Zahl</t>
   </si>
@@ -518,12 +523,21 @@
   </si>
   <si>
     <t>Gruppe5</t>
+  </si>
+  <si>
+    <t>Typ</t>
+  </si>
+  <si>
+    <t>crs</t>
+  </si>
+  <si>
+    <t>grp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
@@ -567,7 +581,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -578,6 +592,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFDCE6F1"/>
         <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -604,7 +624,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -619,6 +639,7 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1901,7 +1922,7 @@
   <dimension ref="A1:P8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1967,7 +1988,9 @@
       <c r="O1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="P1" s="7"/>
+      <c r="P1" s="12" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -2015,11 +2038,13 @@
       <c r="O2" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="P2" s="10"/>
+      <c r="P2" s="10" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>28</v>
@@ -2028,7 +2053,7 @@
         <v>22</v>
       </c>
       <c r="D3">
-        <v>65</v>
+        <v>1</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3" t="s">
@@ -2053,12 +2078,11 @@
       <c r="M3" s="8"/>
       <c r="N3" s="6"/>
       <c r="O3" s="8"/>
-      <c r="P3" s="10"/>
+      <c r="P3" s="10" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>112</v>
-      </c>
       <c r="B4" s="3" t="s">
         <v>29</v>
       </c>
@@ -2066,7 +2090,7 @@
         <v>29</v>
       </c>
       <c r="D4">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3" t="s">
@@ -2099,11 +2123,13 @@
       <c r="O4" s="9">
         <v>0.99998842592592585</v>
       </c>
-      <c r="P4" s="10"/>
+      <c r="P4" s="10" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>113</v>
+        <v>85</v>
       </c>
       <c r="B5" t="s">
         <v>30</v>
@@ -2112,7 +2138,7 @@
         <v>30</v>
       </c>
       <c r="D5">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>23</v>
@@ -2144,11 +2170,13 @@
       <c r="O5" s="9">
         <v>0.99998842592592585</v>
       </c>
-      <c r="P5" s="10"/>
+      <c r="P5" s="10" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>114</v>
+        <v>86</v>
       </c>
       <c r="B6" t="s">
         <v>31</v>
@@ -2157,7 +2185,7 @@
         <v>31</v>
       </c>
       <c r="D6">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>23</v>
@@ -2189,11 +2217,13 @@
       <c r="O6" s="9">
         <v>0.99998842592592585</v>
       </c>
-      <c r="P6" s="10"/>
+      <c r="P6" s="10" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>115</v>
+        <v>87</v>
       </c>
       <c r="B7" t="s">
         <v>32</v>
@@ -2202,7 +2232,7 @@
         <v>32</v>
       </c>
       <c r="D7">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>23</v>
@@ -2234,11 +2264,13 @@
       <c r="O7" s="9">
         <v>0.99998842592592585</v>
       </c>
-      <c r="P7" s="10"/>
+      <c r="P7" s="10" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>116</v>
+        <v>88</v>
       </c>
       <c r="B8" t="s">
         <v>33</v>
@@ -2247,7 +2279,7 @@
         <v>33</v>
       </c>
       <c r="D8">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>23</v>
@@ -2279,13 +2311,15 @@
       <c r="O8" s="9">
         <v>0.99998842592592585</v>
       </c>
-      <c r="P8" s="10"/>
+      <c r="P8" s="10" t="s">
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>